<commit_message>
Upload til SharePoint Testsite
</commit_message>
<xml_diff>
--- a/Indsender_emails.xlsx
+++ b/Indsender_emails.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Indsender emails" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Indsender emails" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -433,7 +433,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B48"/>
+  <dimension ref="A1:B51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -461,562 +461,598 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>S2026-2651</t>
+          <t>S2026-3001</t>
         </is>
       </c>
       <c r="B2" s="2" t="inlineStr">
         <is>
-          <t>mio@huscompagniet.dk</t>
+          <t>ufda@aarhus.dk</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>S2026-691</t>
+          <t>S2026-2651</t>
         </is>
       </c>
       <c r="B3" s="2" t="inlineStr">
         <is>
-          <t>tymurtym40@yahoo.com</t>
+          <t>mio@huscompagniet.dk</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="inlineStr">
         <is>
-          <t>S2025-87195</t>
+          <t>S2026-691</t>
         </is>
       </c>
       <c r="B4" s="2" t="inlineStr">
         <is>
-          <t>mhh-90@hotmail.com</t>
+          <t>tymurtym40@yahoo.com</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="inlineStr">
         <is>
-          <t>S2025-86002</t>
+          <t>S2025-87195</t>
         </is>
       </c>
       <c r="B5" s="2" t="inlineStr">
         <is>
-          <t>vic@jdh-byg.dk</t>
+          <t>mhh-90@hotmail.com</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="inlineStr">
         <is>
-          <t>S2025-85548</t>
+          <t>S2025-86002</t>
         </is>
       </c>
       <c r="B6" s="2" t="inlineStr">
         <is>
-          <t>cmp@visionarkitekter.dk</t>
+          <t>vic@jdh-byg.dk</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="2" t="inlineStr">
         <is>
-          <t>S2025-84319</t>
+          <t>S2025-85548</t>
         </is>
       </c>
       <c r="B7" s="2" t="inlineStr">
         <is>
-          <t>runebossen1@gmail.com</t>
+          <t>cmp@visionarkitekter.dk</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="2" t="inlineStr">
         <is>
-          <t>S2025-84222</t>
+          <t>S2025-84319</t>
         </is>
       </c>
       <c r="B8" s="2" t="inlineStr">
         <is>
-          <t>pil@aarhus.dk</t>
+          <t>runebossen1@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="2" t="inlineStr">
         <is>
-          <t>S2025-84050</t>
+          <t>S2025-84222</t>
         </is>
       </c>
       <c r="B9" s="2" t="inlineStr">
         <is>
-          <t>tp@pwstaal.dk</t>
+          <t>pil@aarhus.dk</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="2" t="inlineStr">
         <is>
-          <t>S2025-83507</t>
+          <t>S2025-84050</t>
         </is>
       </c>
       <c r="B10" s="2" t="inlineStr">
         <is>
-          <t>mn1kurdm@hotmail.com</t>
+          <t>tp@pwstaal.dk</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="2" t="inlineStr">
         <is>
-          <t>S2025-82709</t>
+          <t>S2025-83507</t>
         </is>
       </c>
       <c r="B11" s="2" t="inlineStr">
         <is>
-          <t>as@solarfuture.dk</t>
+          <t>mn1kurdm@hotmail.com</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="2" t="inlineStr">
         <is>
-          <t>S2025-82487</t>
+          <t>S2025-82709</t>
         </is>
       </c>
       <c r="B12" s="2" t="inlineStr">
         <is>
-          <t>ms@et-arkitekter.dk</t>
+          <t>as@solarfuture.dk</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="2" t="inlineStr">
         <is>
-          <t>S2025-82157</t>
+          <t>S2025-82487</t>
         </is>
       </c>
       <c r="B13" s="2" t="inlineStr">
         <is>
-          <t>mlu@procesark.dk</t>
+          <t>ms@et-arkitekter.dk</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="2" t="inlineStr">
         <is>
-          <t>S2025-82152</t>
+          <t>S2025-82367</t>
         </is>
       </c>
       <c r="B14" s="2" t="inlineStr">
         <is>
-          <t>tp@pwstaal.dk</t>
+          <t>uffe@fredens.net</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="2" t="inlineStr">
         <is>
-          <t>S2025-81546</t>
+          <t>S2025-82157</t>
         </is>
       </c>
       <c r="B15" s="2" t="inlineStr">
         <is>
-          <t>ai@ivb.dk</t>
+          <t>mlu@procesark.dk</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="2" t="inlineStr">
         <is>
-          <t>S2025-80845</t>
+          <t>S2025-82152</t>
         </is>
       </c>
       <c r="B16" s="2" t="inlineStr">
         <is>
-          <t>rm@pwstaal.dk</t>
+          <t>tp@pwstaal.dk</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="2" t="inlineStr">
         <is>
-          <t>S2025-80654</t>
+          <t>S2025-81546</t>
         </is>
       </c>
       <c r="B17" s="2" t="inlineStr">
         <is>
-          <t>stinnekrogh@gmail.com</t>
+          <t>ai@ivb.dk</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="2" t="inlineStr">
         <is>
-          <t>S2025-80586</t>
+          <t>S2025-80845</t>
         </is>
       </c>
       <c r="B18" s="2" t="inlineStr">
         <is>
-          <t>malje1986@gmail.com</t>
+          <t>rm@pwstaal.dk</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="2" t="inlineStr">
         <is>
-          <t>S2025-79765</t>
+          <t>S2025-80654</t>
         </is>
       </c>
       <c r="B19" s="2" t="inlineStr">
         <is>
-          <t>lone.ryberg@gmail.com</t>
+          <t>stinnekrogh@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="2" t="inlineStr">
         <is>
-          <t>S2025-79446</t>
+          <t>S2025-80586</t>
         </is>
       </c>
       <c r="B20" s="2" t="inlineStr">
         <is>
-          <t>mhn@arkestate.dk</t>
+          <t>malje1986@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="2" t="inlineStr">
         <is>
-          <t>S2025-78722</t>
+          <t>S2025-79765</t>
         </is>
       </c>
       <c r="B21" s="2" t="inlineStr">
         <is>
-          <t>bjkri@aarhus.dk</t>
+          <t>lone.ryberg@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="2" t="inlineStr">
         <is>
-          <t>S2025-78595</t>
+          <t>S2025-79446</t>
         </is>
       </c>
       <c r="B22" s="2" t="inlineStr">
         <is>
-          <t>jk@nordpil.dk</t>
+          <t>mhn@arkestate.dk</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="2" t="inlineStr">
         <is>
-          <t>S2025-77225</t>
+          <t>S2025-78722</t>
         </is>
       </c>
       <c r="B23" s="2" t="inlineStr">
         <is>
-          <t>tp@pwstaal.dk</t>
+          <t>bjkri@aarhus.dk</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="2" t="inlineStr">
         <is>
-          <t>S2025-77181</t>
+          <t>S2025-78595</t>
         </is>
       </c>
       <c r="B24" s="2" t="inlineStr">
         <is>
-          <t>xiaoxianweng@gmail.com</t>
+          <t>jk@nordpil.dk</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="2" t="inlineStr">
         <is>
-          <t>S2025-76454</t>
+          <t>S2025-77225</t>
         </is>
       </c>
       <c r="B25" s="2" t="inlineStr">
         <is>
-          <t>bjf@a2xj.dk</t>
+          <t>tp@pwstaal.dk</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="2" t="inlineStr">
         <is>
-          <t>S2025-74962</t>
+          <t>S2025-77181</t>
         </is>
       </c>
       <c r="B26" s="2" t="inlineStr">
         <is>
-          <t>heidifrederiksen@hotmail.com</t>
+          <t>xiaoxianweng@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="2" t="inlineStr">
         <is>
-          <t>S2025-74759</t>
+          <t>S2025-76454</t>
         </is>
       </c>
       <c r="B27" s="2" t="inlineStr">
         <is>
-          <t>florin@realservice.dk</t>
+          <t>bjf@a2xj.dk</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="2" t="inlineStr">
         <is>
-          <t>S2025-71862</t>
+          <t>S2025-74962</t>
         </is>
       </c>
       <c r="B28" s="2" t="inlineStr">
         <is>
-          <t>svenneermark@gmail.com</t>
+          <t>heidifrederiksen@hotmail.com</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="2" t="inlineStr">
         <is>
-          <t>S2025-71626</t>
+          <t>S2025-74759</t>
         </is>
       </c>
       <c r="B29" s="2" t="inlineStr">
         <is>
-          <t>ankasp@norlys.dk</t>
+          <t>florin@realservice.dk</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="2" t="inlineStr">
         <is>
-          <t>S2025-63378</t>
+          <t>S2025-71862</t>
         </is>
       </c>
       <c r="B30" s="2" t="inlineStr">
         <is>
-          <t>lpk@onlinebyggetilladelse.dk</t>
+          <t>svenneermark@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="2" t="inlineStr">
         <is>
-          <t>S2025-63355</t>
+          <t>S2025-71626</t>
         </is>
       </c>
       <c r="B31" s="2" t="inlineStr">
         <is>
-          <t>rel@hph-totalbyg.dk</t>
+          <t>ankasp@norlys.dk</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="2" t="inlineStr">
         <is>
-          <t>S2025-61348</t>
+          <t>S2025-68291</t>
         </is>
       </c>
       <c r="B32" s="2" t="inlineStr">
         <is>
-          <t>Helene.Hansen@aarhusvand.dk</t>
+          <t>line.bak.elleskov@danbolig.dk</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="2" t="inlineStr">
         <is>
-          <t>S2025-60684</t>
+          <t>S2025-63378</t>
         </is>
       </c>
       <c r="B33" s="2" t="inlineStr">
         <is>
-          <t>andreas@kops360.dk</t>
+          <t>lpk@onlinebyggetilladelse.dk</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="2" t="inlineStr">
         <is>
-          <t>S2025-60668</t>
+          <t>S2025-63355</t>
         </is>
       </c>
       <c r="B34" s="2" t="inlineStr">
         <is>
-          <t>hesa@kglteater.dk</t>
+          <t>rel@hph-totalbyg.dk</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="2" t="inlineStr">
         <is>
-          <t>S2025-59073</t>
+          <t>S2025-61348</t>
         </is>
       </c>
       <c r="B35" s="2" t="inlineStr">
         <is>
-          <t>hfhumlehaven@gmail.com</t>
+          <t>Helene.Hansen@aarhusvand.dk</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="2" t="inlineStr">
         <is>
-          <t>S2025-56760</t>
+          <t>S2025-60684</t>
         </is>
       </c>
       <c r="B36" s="2" t="inlineStr">
         <is>
-          <t>sk@kjellerup.eu</t>
+          <t>andreas@kops360.dk</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="2" t="inlineStr">
         <is>
-          <t>S2025-56632</t>
+          <t>S2025-60668</t>
         </is>
       </c>
       <c r="B37" s="2" t="inlineStr">
         <is>
-          <t>casper@stenhoj-husene.dk</t>
+          <t>hesa@kglteater.dk</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="2" t="inlineStr">
         <is>
-          <t>S2025-54532</t>
+          <t>S2025-59073</t>
         </is>
       </c>
       <c r="B38" s="2" t="inlineStr">
         <is>
-          <t>mettevoigt@outlook.com</t>
+          <t>hfhumlehaven@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="2" t="inlineStr">
         <is>
-          <t>S2025-53815</t>
+          <t>S2025-56760</t>
         </is>
       </c>
       <c r="B39" s="2" t="inlineStr">
         <is>
-          <t>sarah_eyad@hotmail.com</t>
+          <t>sk@kjellerup.eu</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="2" t="inlineStr">
         <is>
-          <t>S2025-53405</t>
+          <t>S2025-56632</t>
         </is>
       </c>
       <c r="B40" s="2" t="inlineStr">
         <is>
-          <t>ml@nodo.dk</t>
+          <t>casper@stenhoj-husene.dk</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="2" t="inlineStr">
         <is>
-          <t>S2025-52476</t>
+          <t>S2025-54532</t>
         </is>
       </c>
       <c r="B41" s="2" t="inlineStr">
         <is>
-          <t>hyldgaard@fibermail.dk</t>
+          <t>mettevoigt@outlook.com</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="2" t="inlineStr">
         <is>
-          <t>S2025-47889</t>
+          <t>S2025-53815</t>
         </is>
       </c>
       <c r="B42" s="2" t="inlineStr">
         <is>
-          <t>ac@cfmoller.com</t>
+          <t>sarah_eyad@hotmail.com</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="2" t="inlineStr">
         <is>
-          <t>S2025-32455</t>
+          <t>S2025-53405</t>
         </is>
       </c>
       <c r="B43" s="2" t="inlineStr">
         <is>
-          <t>kg@kristiangislason.dk</t>
+          <t>ml@nodo.dk</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="2" t="inlineStr">
         <is>
-          <t>S2025-31869</t>
+          <t>S2025-52476</t>
         </is>
       </c>
       <c r="B44" s="2" t="inlineStr">
         <is>
-          <t>ebk@clevrcar.dk</t>
+          <t>hyldgaard@fibermail.dk</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="2" t="inlineStr">
         <is>
-          <t>S2025-14575</t>
+          <t>S2025-47889</t>
         </is>
       </c>
       <c r="B45" s="2" t="inlineStr">
         <is>
-          <t>Morten.Krogh@hk.dk</t>
+          <t>ac@cfmoller.com</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="2" t="inlineStr">
         <is>
-          <t>S2025-2284</t>
+          <t>S2025-32455</t>
         </is>
       </c>
       <c r="B46" s="2" t="inlineStr">
         <is>
-          <t>rp@skikarkitekter.dk</t>
+          <t>kg@kristiangislason.dk</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="2" t="inlineStr">
         <is>
-          <t>S2024-34950</t>
+          <t>S2025-31869</t>
         </is>
       </c>
       <c r="B47" s="2" t="inlineStr">
         <is>
-          <t>laura@looparchitects.dk</t>
+          <t>ebk@clevrcar.dk</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="2" t="inlineStr">
         <is>
+          <t>S2025-14575</t>
+        </is>
+      </c>
+      <c r="B48" s="2" t="inlineStr">
+        <is>
+          <t>Morten.Krogh@hk.dk</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="2" t="inlineStr">
+        <is>
+          <t>S2025-2284</t>
+        </is>
+      </c>
+      <c r="B49" s="2" t="inlineStr">
+        <is>
+          <t>rp@skikarkitekter.dk</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="2" t="inlineStr">
+        <is>
+          <t>S2024-34950</t>
+        </is>
+      </c>
+      <c r="B50" s="2" t="inlineStr">
+        <is>
+          <t>laura@looparchitects.dk</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="2" t="inlineStr">
+        <is>
           <t>S2023-33795</t>
         </is>
       </c>
-      <c r="B48" s="2" t="inlineStr">
+      <c r="B51" s="2" t="inlineStr">
         <is>
           <t>jl@vming.dk</t>
         </is>

</xml_diff>